<commit_message>
updata DIC Lab2 and Algorithm Lab2
</commit_message>
<xml_diff>
--- a/DIC/Lab2/Task4/task4.xlsx
+++ b/DIC/Lab2/Task4/task4.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:R27"/>
+  <dimension ref="A1:R52"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -530,49 +530,49 @@
         <v>0.5</v>
       </c>
       <c r="B2" t="n">
-        <v>1.353e-11</v>
+        <v>1.41e-11</v>
       </c>
       <c r="C2" t="n">
-        <v>1.234e-11</v>
+        <v>1.292e-11</v>
       </c>
       <c r="D2" t="n">
-        <v>1.294e-11</v>
+        <v>1.351e-11</v>
       </c>
       <c r="E2" t="n">
-        <v>9.709000000000001e-12</v>
+        <v>9.633e-12</v>
       </c>
       <c r="F2" t="n">
-        <v>9.879e-12</v>
+        <v>9.676e-12</v>
       </c>
       <c r="G2" t="n">
-        <v>9.794e-12</v>
+        <v>9.655e-12</v>
       </c>
       <c r="H2" t="n">
-        <v>1.035e-11</v>
+        <v>1.047e-11</v>
       </c>
       <c r="I2" t="n">
-        <v>9.927e-12</v>
+        <v>9.870000000000001e-12</v>
       </c>
       <c r="J2" t="n">
-        <v>1.014e-11</v>
+        <v>1.017e-11</v>
       </c>
       <c r="K2" t="n">
-        <v>6.975e-12</v>
+        <v>1.149e-11</v>
       </c>
       <c r="L2" t="n">
-        <v>9.557999999999999e-12</v>
+        <v>1.098e-11</v>
       </c>
       <c r="M2" t="n">
-        <v>8.266999999999999e-12</v>
+        <v>1.123e-11</v>
       </c>
       <c r="N2" t="n">
-        <v>4.114e-11</v>
+        <v>4.456e-11</v>
       </c>
       <c r="O2" t="n">
-        <v>-1.274e-05</v>
+        <v>-2.023e-05</v>
       </c>
       <c r="P2" t="n">
-        <v>2.155e-26</v>
+        <v>4.018e-26</v>
       </c>
       <c r="Q2" t="n">
         <v>25</v>
@@ -586,49 +586,49 @@
         <v>0.52</v>
       </c>
       <c r="B3" t="n">
-        <v>1.322e-11</v>
+        <v>1.359e-11</v>
       </c>
       <c r="C3" t="n">
-        <v>1.194e-11</v>
+        <v>1.246e-11</v>
       </c>
       <c r="D3" t="n">
-        <v>1.258e-11</v>
+        <v>1.302e-11</v>
       </c>
       <c r="E3" t="n">
-        <v>9.178e-12</v>
+        <v>9.039e-12</v>
       </c>
       <c r="F3" t="n">
-        <v>9.095e-12</v>
+        <v>9.060000000000001e-12</v>
       </c>
       <c r="G3" t="n">
-        <v>9.136e-12</v>
+        <v>9.05e-12</v>
       </c>
       <c r="H3" t="n">
-        <v>9.949e-12</v>
+        <v>9.862e-12</v>
       </c>
       <c r="I3" t="n">
-        <v>9.397e-12</v>
+        <v>9.297e-12</v>
       </c>
       <c r="J3" t="n">
-        <v>9.673e-12</v>
+        <v>9.580000000000001e-12</v>
       </c>
       <c r="K3" t="n">
-        <v>6.654e-12</v>
+        <v>1.087e-11</v>
       </c>
       <c r="L3" t="n">
-        <v>8.882999999999999e-12</v>
+        <v>1.035e-11</v>
       </c>
       <c r="M3" t="n">
-        <v>7.769000000000001e-12</v>
+        <v>1.061e-11</v>
       </c>
       <c r="N3" t="n">
-        <v>3.915e-11</v>
+        <v>4.226e-11</v>
       </c>
       <c r="O3" t="n">
-        <v>-1.403e-05</v>
+        <v>-2.211e-05</v>
       </c>
       <c r="P3" t="n">
-        <v>2.151e-26</v>
+        <v>3.95e-26</v>
       </c>
       <c r="Q3" t="n">
         <v>25</v>
@@ -642,49 +642,49 @@
         <v>0.54</v>
       </c>
       <c r="B4" t="n">
-        <v>1.276e-11</v>
+        <v>1.313e-11</v>
       </c>
       <c r="C4" t="n">
-        <v>1.165e-11</v>
+        <v>1.205e-11</v>
       </c>
       <c r="D4" t="n">
-        <v>1.22e-11</v>
+        <v>1.259e-11</v>
       </c>
       <c r="E4" t="n">
-        <v>8.534999999999999e-12</v>
+        <v>8.584e-12</v>
       </c>
       <c r="F4" t="n">
-        <v>8.501e-12</v>
+        <v>8.529e-12</v>
       </c>
       <c r="G4" t="n">
-        <v>8.518000000000001e-12</v>
+        <v>8.557000000000001e-12</v>
       </c>
       <c r="H4" t="n">
-        <v>9.482e-12</v>
+        <v>9.35e-12</v>
       </c>
       <c r="I4" t="n">
-        <v>9.018999999999999e-12</v>
+        <v>8.805999999999999e-12</v>
       </c>
       <c r="J4" t="n">
-        <v>9.25e-12</v>
+        <v>9.078e-12</v>
       </c>
       <c r="K4" t="n">
-        <v>6.115e-12</v>
+        <v>1.034e-11</v>
       </c>
       <c r="L4" t="n">
-        <v>8.401e-12</v>
+        <v>9.831999999999999e-12</v>
       </c>
       <c r="M4" t="n">
-        <v>7.258e-12</v>
+        <v>1.008e-11</v>
       </c>
       <c r="N4" t="n">
-        <v>3.723e-11</v>
+        <v>4.031e-11</v>
       </c>
       <c r="O4" t="n">
-        <v>-1.53e-05</v>
+        <v>-2.411e-05</v>
       </c>
       <c r="P4" t="n">
-        <v>2.121e-26</v>
+        <v>3.917e-26</v>
       </c>
       <c r="Q4" t="n">
         <v>25</v>
@@ -698,49 +698,49 @@
         <v>0.5600000000000001</v>
       </c>
       <c r="B5" t="n">
-        <v>1.258e-11</v>
+        <v>1.275e-11</v>
       </c>
       <c r="C5" t="n">
-        <v>1.135e-11</v>
+        <v>1.165e-11</v>
       </c>
       <c r="D5" t="n">
-        <v>1.196e-11</v>
+        <v>1.22e-11</v>
       </c>
       <c r="E5" t="n">
-        <v>8.242e-12</v>
+        <v>8.195000000000001e-12</v>
       </c>
       <c r="F5" t="n">
         <v>8.061e-12</v>
       </c>
       <c r="G5" t="n">
-        <v>8.150999999999999e-12</v>
+        <v>8.127999999999999e-12</v>
       </c>
       <c r="H5" t="n">
-        <v>9.046e-12</v>
+        <v>8.908999999999999e-12</v>
       </c>
       <c r="I5" t="n">
-        <v>8.495e-12</v>
+        <v>8.385e-12</v>
       </c>
       <c r="J5" t="n">
-        <v>8.771e-12</v>
+        <v>8.647000000000001e-12</v>
       </c>
       <c r="K5" t="n">
-        <v>6.029e-12</v>
+        <v>9.886e-12</v>
       </c>
       <c r="L5" t="n">
-        <v>8e-12</v>
+        <v>9.366e-12</v>
       </c>
       <c r="M5" t="n">
-        <v>7.014e-12</v>
+        <v>9.626e-12</v>
       </c>
       <c r="N5" t="n">
-        <v>3.59e-11</v>
+        <v>3.86e-11</v>
       </c>
       <c r="O5" t="n">
-        <v>-1.665e-05</v>
+        <v>-2.62e-05</v>
       </c>
       <c r="P5" t="n">
-        <v>2.146e-26</v>
+        <v>3.904000000000001e-26</v>
       </c>
       <c r="Q5" t="n">
         <v>25</v>
@@ -754,49 +754,49 @@
         <v>0.58</v>
       </c>
       <c r="B6" t="n">
-        <v>1.19e-11</v>
+        <v>1.24e-11</v>
       </c>
       <c r="C6" t="n">
-        <v>1.114e-11</v>
+        <v>1.129e-11</v>
       </c>
       <c r="D6" t="n">
-        <v>1.152e-11</v>
+        <v>1.184e-11</v>
       </c>
       <c r="E6" t="n">
-        <v>7.738e-12</v>
+        <v>7.862e-12</v>
       </c>
       <c r="F6" t="n">
-        <v>7.719e-12</v>
+        <v>7.688e-12</v>
       </c>
       <c r="G6" t="n">
-        <v>7.727999999999999e-12</v>
+        <v>7.775e-12</v>
       </c>
       <c r="H6" t="n">
-        <v>8.662e-12</v>
+        <v>8.523e-12</v>
       </c>
       <c r="I6" t="n">
-        <v>8.193e-12</v>
+        <v>8.019e-12</v>
       </c>
       <c r="J6" t="n">
-        <v>8.427999999999999e-12</v>
+        <v>8.271e-12</v>
       </c>
       <c r="K6" t="n">
-        <v>5.719e-12</v>
+        <v>9.492999999999999e-12</v>
       </c>
       <c r="L6" t="n">
-        <v>7.682999999999999e-12</v>
+        <v>8.975e-12</v>
       </c>
       <c r="M6" t="n">
-        <v>6.701e-12</v>
+        <v>9.234e-12</v>
       </c>
       <c r="N6" t="n">
-        <v>3.437e-11</v>
+        <v>3.712e-11</v>
       </c>
       <c r="O6" t="n">
-        <v>-1.812e-05</v>
+        <v>-2.839e-05</v>
       </c>
       <c r="P6" t="n">
-        <v>2.141e-26</v>
+        <v>3.913e-26</v>
       </c>
       <c r="Q6" t="n">
         <v>25</v>
@@ -810,49 +810,49 @@
         <v>0.6</v>
       </c>
       <c r="B7" t="n">
-        <v>1.17e-11</v>
+        <v>1.206e-11</v>
       </c>
       <c r="C7" t="n">
-        <v>1.078e-11</v>
+        <v>1.097e-11</v>
       </c>
       <c r="D7" t="n">
-        <v>1.124e-11</v>
+        <v>1.151e-11</v>
       </c>
       <c r="E7" t="n">
-        <v>7.568e-12</v>
+        <v>7.571e-12</v>
       </c>
       <c r="F7" t="n">
-        <v>7.394e-12</v>
+        <v>7.362999999999999e-12</v>
       </c>
       <c r="G7" t="n">
-        <v>7.481e-12</v>
+        <v>7.467e-12</v>
       </c>
       <c r="H7" t="n">
-        <v>8.352e-12</v>
+        <v>8.187e-12</v>
       </c>
       <c r="I7" t="n">
-        <v>7.927e-12</v>
+        <v>7.7e-12</v>
       </c>
       <c r="J7" t="n">
-        <v>8.139e-12</v>
+        <v>7.943999999999999e-12</v>
       </c>
       <c r="K7" t="n">
-        <v>5.428e-12</v>
+        <v>9.15e-12</v>
       </c>
       <c r="L7" t="n">
-        <v>7.122e-12</v>
+        <v>8.616e-12</v>
       </c>
       <c r="M7" t="n">
-        <v>6.275e-12</v>
+        <v>8.882999999999999e-12</v>
       </c>
       <c r="N7" t="n">
-        <v>3.314e-11</v>
+        <v>3.581e-11</v>
       </c>
       <c r="O7" t="n">
-        <v>-1.958e-05</v>
+        <v>-3.069e-05</v>
       </c>
       <c r="P7" t="n">
-        <v>2.149e-26</v>
+        <v>3.935e-26</v>
       </c>
       <c r="Q7" t="n">
         <v>25</v>
@@ -866,49 +866,49 @@
         <v>0.62</v>
       </c>
       <c r="B8" t="n">
-        <v>1.137e-11</v>
+        <v>1.176e-11</v>
       </c>
       <c r="C8" t="n">
-        <v>1.035e-11</v>
+        <v>1.068e-11</v>
       </c>
       <c r="D8" t="n">
-        <v>1.086e-11</v>
+        <v>1.122e-11</v>
       </c>
       <c r="E8" t="n">
-        <v>7.251e-12</v>
+        <v>7.309e-12</v>
       </c>
       <c r="F8" t="n">
-        <v>7.105e-12</v>
+        <v>7.065e-12</v>
       </c>
       <c r="G8" t="n">
-        <v>7.178e-12</v>
+        <v>7.187e-12</v>
       </c>
       <c r="H8" t="n">
-        <v>8.065e-12</v>
+        <v>7.895000000000001e-12</v>
       </c>
       <c r="I8" t="n">
-        <v>7.598000000000001e-12</v>
+        <v>7.421000000000001e-12</v>
       </c>
       <c r="J8" t="n">
-        <v>7.832e-12</v>
+        <v>7.658e-12</v>
       </c>
       <c r="K8" t="n">
-        <v>5.415e-12</v>
+        <v>8.842e-12</v>
       </c>
       <c r="L8" t="n">
-        <v>6.855e-12</v>
+        <v>8.307e-12</v>
       </c>
       <c r="M8" t="n">
-        <v>6.135e-12</v>
+        <v>8.575e-12</v>
       </c>
       <c r="N8" t="n">
-        <v>3.201e-11</v>
+        <v>3.464e-11</v>
       </c>
       <c r="O8" t="n">
-        <v>-2.125e-05</v>
+        <v>-3.311e-05</v>
       </c>
       <c r="P8" t="n">
-        <v>2.177e-26</v>
+        <v>3.972000000000001e-26</v>
       </c>
       <c r="Q8" t="n">
         <v>25</v>
@@ -922,49 +922,49 @@
         <v>0.64</v>
       </c>
       <c r="B9" t="n">
-        <v>1.118e-11</v>
+        <v>1.148e-11</v>
       </c>
       <c r="C9" t="n">
-        <v>1.032e-11</v>
+        <v>1.04e-11</v>
       </c>
       <c r="D9" t="n">
-        <v>1.075e-11</v>
+        <v>1.094e-11</v>
       </c>
       <c r="E9" t="n">
-        <v>6.976e-12</v>
+        <v>7.096e-12</v>
       </c>
       <c r="F9" t="n">
-        <v>6.845e-12</v>
+        <v>6.835e-12</v>
       </c>
       <c r="G9" t="n">
-        <v>6.91e-12</v>
+        <v>6.966e-12</v>
       </c>
       <c r="H9" t="n">
-        <v>7.73e-12</v>
+        <v>7.632e-12</v>
       </c>
       <c r="I9" t="n">
-        <v>7.412e-12</v>
+        <v>7.169e-12</v>
       </c>
       <c r="J9" t="n">
-        <v>7.571e-12</v>
+        <v>7.401e-12</v>
       </c>
       <c r="K9" t="n">
-        <v>5.205e-12</v>
+        <v>8.562e-12</v>
       </c>
       <c r="L9" t="n">
-        <v>6.692e-12</v>
+        <v>8.043e-12</v>
       </c>
       <c r="M9" t="n">
-        <v>5.949e-12</v>
+        <v>8.303e-12</v>
       </c>
       <c r="N9" t="n">
-        <v>3.118e-11</v>
+        <v>3.361e-11</v>
       </c>
       <c r="O9" t="n">
-        <v>-2.299e-05</v>
+        <v>-3.562e-05</v>
       </c>
       <c r="P9" t="n">
-        <v>2.235e-26</v>
+        <v>4.023e-26</v>
       </c>
       <c r="Q9" t="n">
         <v>25</v>
@@ -978,49 +978,49 @@
         <v>0.66</v>
       </c>
       <c r="B10" t="n">
-        <v>1.09e-11</v>
+        <v>1.122e-11</v>
       </c>
       <c r="C10" t="n">
-        <v>1.012e-11</v>
+        <v>1.014e-11</v>
       </c>
       <c r="D10" t="n">
-        <v>1.051e-11</v>
+        <v>1.068e-11</v>
       </c>
       <c r="E10" t="n">
-        <v>6.549e-12</v>
+        <v>6.901e-12</v>
       </c>
       <c r="F10" t="n">
-        <v>6.481e-12</v>
+        <v>6.615e-12</v>
       </c>
       <c r="G10" t="n">
-        <v>6.515e-12</v>
+        <v>6.758e-12</v>
       </c>
       <c r="H10" t="n">
-        <v>7.559e-12</v>
+        <v>7.398000000000001e-12</v>
       </c>
       <c r="I10" t="n">
-        <v>7.215e-12</v>
+        <v>6.944e-12</v>
       </c>
       <c r="J10" t="n">
-        <v>7.387e-12</v>
+        <v>7.171e-12</v>
       </c>
       <c r="K10" t="n">
-        <v>5.01e-12</v>
+        <v>8.319e-12</v>
       </c>
       <c r="L10" t="n">
-        <v>6.431e-12</v>
+        <v>7.782999999999999e-12</v>
       </c>
       <c r="M10" t="n">
-        <v>5.72e-12</v>
+        <v>8.051e-12</v>
       </c>
       <c r="N10" t="n">
-        <v>3.013e-11</v>
+        <v>3.266e-11</v>
       </c>
       <c r="O10" t="n">
-        <v>-2.469e-05</v>
+        <v>-3.825e-05</v>
       </c>
       <c r="P10" t="n">
-        <v>2.242e-26</v>
+        <v>4.080000000000001e-26</v>
       </c>
       <c r="Q10" t="n">
         <v>25</v>
@@ -1034,49 +1034,49 @@
         <v>0.68</v>
       </c>
       <c r="B11" t="n">
-        <v>1.076e-11</v>
+        <v>1.098e-11</v>
       </c>
       <c r="C11" t="n">
-        <v>1.005e-11</v>
+        <v>9.924e-12</v>
       </c>
       <c r="D11" t="n">
-        <v>1.04e-11</v>
+        <v>1.045e-11</v>
       </c>
       <c r="E11" t="n">
-        <v>6.256e-12</v>
+        <v>6.726e-12</v>
       </c>
       <c r="F11" t="n">
-        <v>6.25e-12</v>
+        <v>6.424e-12</v>
       </c>
       <c r="G11" t="n">
-        <v>6.253e-12</v>
+        <v>6.575e-12</v>
       </c>
       <c r="H11" t="n">
-        <v>7.325e-12</v>
+        <v>7.18e-12</v>
       </c>
       <c r="I11" t="n">
-        <v>6.985e-12</v>
+        <v>6.737e-12</v>
       </c>
       <c r="J11" t="n">
-        <v>7.155e-12</v>
+        <v>6.958e-12</v>
       </c>
       <c r="K11" t="n">
-        <v>4.961e-12</v>
+        <v>8.113e-12</v>
       </c>
       <c r="L11" t="n">
-        <v>6.297e-12</v>
+        <v>7.572e-12</v>
       </c>
       <c r="M11" t="n">
-        <v>5.629e-12</v>
+        <v>7.843e-12</v>
       </c>
       <c r="N11" t="n">
-        <v>2.944e-11</v>
+        <v>3.183e-11</v>
       </c>
       <c r="O11" t="n">
-        <v>-2.653e-05</v>
+        <v>-4.098e-05</v>
       </c>
       <c r="P11" t="n">
-        <v>2.299e-26</v>
+        <v>4.152000000000001e-26</v>
       </c>
       <c r="Q11" t="n">
         <v>25</v>
@@ -1090,49 +1090,49 @@
         <v>0.7</v>
       </c>
       <c r="B12" t="n">
-        <v>1.078e-11</v>
+        <v>1.077e-11</v>
       </c>
       <c r="C12" t="n">
-        <v>9.772e-12</v>
+        <v>9.680000000000001e-12</v>
       </c>
       <c r="D12" t="n">
-        <v>1.028e-11</v>
+        <v>1.022e-11</v>
       </c>
       <c r="E12" t="n">
-        <v>6.288e-12</v>
+        <v>6.576e-12</v>
       </c>
       <c r="F12" t="n">
-        <v>5.996e-12</v>
+        <v>6.246e-12</v>
       </c>
       <c r="G12" t="n">
-        <v>6.142e-12</v>
+        <v>6.411e-12</v>
       </c>
       <c r="H12" t="n">
-        <v>7.198e-12</v>
+        <v>6.987e-12</v>
       </c>
       <c r="I12" t="n">
-        <v>6.718e-12</v>
+        <v>6.561e-12</v>
       </c>
       <c r="J12" t="n">
-        <v>6.958e-12</v>
+        <v>6.774e-12</v>
       </c>
       <c r="K12" t="n">
-        <v>5.033e-12</v>
+        <v>7.913e-12</v>
       </c>
       <c r="L12" t="n">
-        <v>6.207e-12</v>
+        <v>7.371e-12</v>
       </c>
       <c r="M12" t="n">
-        <v>5.62e-12</v>
+        <v>7.642e-12</v>
       </c>
       <c r="N12" t="n">
-        <v>2.9e-11</v>
+        <v>3.105e-11</v>
       </c>
       <c r="O12" t="n">
-        <v>-2.853e-05</v>
+        <v>-4.385e-05</v>
       </c>
       <c r="P12" t="n">
-        <v>2.399e-26</v>
+        <v>4.228e-26</v>
       </c>
       <c r="Q12" t="n">
         <v>25</v>
@@ -1146,49 +1146,49 @@
         <v>0.72</v>
       </c>
       <c r="B13" t="n">
-        <v>1.032e-11</v>
+        <v>1.057e-11</v>
       </c>
       <c r="C13" t="n">
-        <v>9.685e-12</v>
+        <v>9.480000000000001e-12</v>
       </c>
       <c r="D13" t="n">
-        <v>9.999999999999999e-12</v>
+        <v>1.002e-11</v>
       </c>
       <c r="E13" t="n">
-        <v>5.95e-12</v>
+        <v>6.437e-12</v>
       </c>
       <c r="F13" t="n">
-        <v>5.951e-12</v>
+        <v>6.093e-12</v>
       </c>
       <c r="G13" t="n">
-        <v>5.95e-12</v>
+        <v>6.265e-12</v>
       </c>
       <c r="H13" t="n">
-        <v>6.992e-12</v>
+        <v>6.829e-12</v>
       </c>
       <c r="I13" t="n">
-        <v>6.544e-12</v>
+        <v>6.393e-12</v>
       </c>
       <c r="J13" t="n">
-        <v>6.768e-12</v>
+        <v>6.611e-12</v>
       </c>
       <c r="K13" t="n">
-        <v>4.86e-12</v>
+        <v>7.73e-12</v>
       </c>
       <c r="L13" t="n">
-        <v>6.026e-12</v>
+        <v>7.191e-12</v>
       </c>
       <c r="M13" t="n">
-        <v>5.443e-12</v>
+        <v>7.459999999999999e-12</v>
       </c>
       <c r="N13" t="n">
-        <v>2.816e-11</v>
+        <v>3.036e-11</v>
       </c>
       <c r="O13" t="n">
-        <v>-3.07e-05</v>
+        <v>-4.681e-05</v>
       </c>
       <c r="P13" t="n">
-        <v>2.435e-26</v>
+        <v>4.314000000000001e-26</v>
       </c>
       <c r="Q13" t="n">
         <v>25</v>
@@ -1202,49 +1202,49 @@
         <v>0.74</v>
       </c>
       <c r="B14" t="n">
-        <v>1.039e-11</v>
+        <v>1.038e-11</v>
       </c>
       <c r="C14" t="n">
-        <v>9.144000000000001e-12</v>
+        <v>9.291e-12</v>
       </c>
       <c r="D14" t="n">
-        <v>9.768e-12</v>
+        <v>9.833e-12</v>
       </c>
       <c r="E14" t="n">
-        <v>6.297e-12</v>
+        <v>6.31e-12</v>
       </c>
       <c r="F14" t="n">
-        <v>5.619e-12</v>
+        <v>5.956e-12</v>
       </c>
       <c r="G14" t="n">
-        <v>5.958e-12</v>
+        <v>6.133e-12</v>
       </c>
       <c r="H14" t="n">
-        <v>6.883e-12</v>
+        <v>6.667e-12</v>
       </c>
       <c r="I14" t="n">
-        <v>6.435e-12</v>
+        <v>6.244e-12</v>
       </c>
       <c r="J14" t="n">
-        <v>6.659e-12</v>
+        <v>6.456e-12</v>
       </c>
       <c r="K14" t="n">
-        <v>4.736e-12</v>
+        <v>7.574e-12</v>
       </c>
       <c r="L14" t="n">
-        <v>5.783e-12</v>
+        <v>7.023e-12</v>
       </c>
       <c r="M14" t="n">
-        <v>5.26e-12</v>
+        <v>7.298000000000001e-12</v>
       </c>
       <c r="N14" t="n">
-        <v>2.765e-11</v>
+        <v>2.972e-11</v>
       </c>
       <c r="O14" t="n">
-        <v>-3.277e-05</v>
+        <v>-4.989e-05</v>
       </c>
       <c r="P14" t="n">
-        <v>2.505e-26</v>
+        <v>4.407e-26</v>
       </c>
       <c r="Q14" t="n">
         <v>25</v>
@@ -1258,49 +1258,49 @@
         <v>0.76</v>
       </c>
       <c r="B15" t="n">
-        <v>1.002e-11</v>
+        <v>1.02e-11</v>
       </c>
       <c r="C15" t="n">
-        <v>9.275e-12</v>
+        <v>9.131000000000001e-12</v>
       </c>
       <c r="D15" t="n">
-        <v>9.65e-12</v>
+        <v>9.666e-12</v>
       </c>
       <c r="E15" t="n">
-        <v>5.85e-12</v>
+        <v>6.191e-12</v>
       </c>
       <c r="F15" t="n">
-        <v>5.755e-12</v>
+        <v>5.834e-12</v>
       </c>
       <c r="G15" t="n">
-        <v>5.802e-12</v>
+        <v>6.012e-12</v>
       </c>
       <c r="H15" t="n">
-        <v>6.692e-12</v>
+        <v>6.529e-12</v>
       </c>
       <c r="I15" t="n">
-        <v>6.322e-12</v>
+        <v>6.108e-12</v>
       </c>
       <c r="J15" t="n">
-        <v>6.507e-12</v>
+        <v>6.319e-12</v>
       </c>
       <c r="K15" t="n">
-        <v>4.667e-12</v>
+        <v>7.419e-12</v>
       </c>
       <c r="L15" t="n">
-        <v>5.742e-12</v>
+        <v>6.882e-12</v>
       </c>
       <c r="M15" t="n">
-        <v>5.205e-12</v>
+        <v>7.15e-12</v>
       </c>
       <c r="N15" t="n">
-        <v>2.716e-11</v>
+        <v>2.915e-11</v>
       </c>
       <c r="O15" t="n">
-        <v>-3.506e-05</v>
+        <v>-5.309e-05</v>
       </c>
       <c r="P15" t="n">
-        <v>2.587e-26</v>
+        <v>4.51e-26</v>
       </c>
       <c r="Q15" t="n">
         <v>25</v>
@@ -1314,49 +1314,49 @@
         <v>0.78</v>
       </c>
       <c r="B16" t="n">
-        <v>9.883999999999999e-12</v>
+        <v>1.006e-11</v>
       </c>
       <c r="C16" t="n">
-        <v>9.143e-12</v>
+        <v>8.971e-12</v>
       </c>
       <c r="D16" t="n">
-        <v>9.514e-12</v>
+        <v>9.518e-12</v>
       </c>
       <c r="E16" t="n">
-        <v>5.715e-12</v>
+        <v>6.072e-12</v>
       </c>
       <c r="F16" t="n">
-        <v>5.663e-12</v>
+        <v>5.717e-12</v>
       </c>
       <c r="G16" t="n">
-        <v>5.689e-12</v>
+        <v>5.894e-12</v>
       </c>
       <c r="H16" t="n">
-        <v>6.574e-12</v>
+        <v>6.4e-12</v>
       </c>
       <c r="I16" t="n">
-        <v>6.162e-12</v>
+        <v>5.978e-12</v>
       </c>
       <c r="J16" t="n">
-        <v>6.368e-12</v>
+        <v>6.189e-12</v>
       </c>
       <c r="K16" t="n">
-        <v>4.616e-12</v>
+        <v>7.287e-12</v>
       </c>
       <c r="L16" t="n">
-        <v>5.571e-12</v>
+        <v>6.746e-12</v>
       </c>
       <c r="M16" t="n">
-        <v>5.094e-12</v>
+        <v>7.016e-12</v>
       </c>
       <c r="N16" t="n">
-        <v>2.667e-11</v>
+        <v>2.862e-11</v>
       </c>
       <c r="O16" t="n">
-        <v>-3.733e-05</v>
+        <v>-5.642e-05</v>
       </c>
       <c r="P16" t="n">
-        <v>2.655e-26</v>
+        <v>4.621000000000001e-26</v>
       </c>
       <c r="Q16" t="n">
         <v>25</v>
@@ -1370,49 +1370,49 @@
         <v>0.8</v>
       </c>
       <c r="B17" t="n">
-        <v>1.013e-11</v>
+        <v>9.891e-12</v>
       </c>
       <c r="C17" t="n">
-        <v>8.669e-12</v>
+        <v>8.823e-12</v>
       </c>
       <c r="D17" t="n">
-        <v>9.398e-12</v>
+        <v>9.357000000000001e-12</v>
       </c>
       <c r="E17" t="n">
-        <v>6.123e-12</v>
+        <v>5.976e-12</v>
       </c>
       <c r="F17" t="n">
-        <v>5.154e-12</v>
+        <v>5.609e-12</v>
       </c>
       <c r="G17" t="n">
-        <v>5.638e-12</v>
+        <v>5.793e-12</v>
       </c>
       <c r="H17" t="n">
-        <v>6.389e-12</v>
+        <v>6.27e-12</v>
       </c>
       <c r="I17" t="n">
-        <v>5.95e-12</v>
+        <v>5.867e-12</v>
       </c>
       <c r="J17" t="n">
-        <v>6.169e-12</v>
+        <v>6.069e-12</v>
       </c>
       <c r="K17" t="n">
-        <v>4.663e-12</v>
+        <v>7.168e-12</v>
       </c>
       <c r="L17" t="n">
-        <v>5.355e-12</v>
+        <v>6.631e-12</v>
       </c>
       <c r="M17" t="n">
-        <v>5.009e-12</v>
+        <v>6.9e-12</v>
       </c>
       <c r="N17" t="n">
-        <v>2.621e-11</v>
+        <v>2.812e-11</v>
       </c>
       <c r="O17" t="n">
-        <v>-3.979e-05</v>
+        <v>-5.985e-05</v>
       </c>
       <c r="P17" t="n">
-        <v>2.735e-26</v>
+        <v>4.732e-26</v>
       </c>
       <c r="Q17" t="n">
         <v>25</v>
@@ -1426,49 +1426,49 @@
         <v>0.82</v>
       </c>
       <c r="B18" t="n">
-        <v>9.778e-12</v>
+        <v>9.780000000000001e-12</v>
       </c>
       <c r="C18" t="n">
-        <v>8.547000000000001e-12</v>
+        <v>8.682999999999999e-12</v>
       </c>
       <c r="D18" t="n">
-        <v>9.163e-12</v>
+        <v>9.231999999999999e-12</v>
       </c>
       <c r="E18" t="n">
-        <v>6.053e-12</v>
+        <v>5.881e-12</v>
       </c>
       <c r="F18" t="n">
-        <v>5.279e-12</v>
+        <v>5.512e-12</v>
       </c>
       <c r="G18" t="n">
-        <v>5.666e-12</v>
+        <v>5.697e-12</v>
       </c>
       <c r="H18" t="n">
-        <v>6.271e-12</v>
+        <v>6.16e-12</v>
       </c>
       <c r="I18" t="n">
-        <v>5.853e-12</v>
+        <v>5.76e-12</v>
       </c>
       <c r="J18" t="n">
-        <v>6.062e-12</v>
+        <v>5.96e-12</v>
       </c>
       <c r="K18" t="n">
-        <v>4.665e-12</v>
+        <v>7.052e-12</v>
       </c>
       <c r="L18" t="n">
-        <v>5.254e-12</v>
+        <v>6.517e-12</v>
       </c>
       <c r="M18" t="n">
-        <v>4.959e-12</v>
+        <v>6.785e-12</v>
       </c>
       <c r="N18" t="n">
-        <v>2.585e-11</v>
+        <v>2.767e-11</v>
       </c>
       <c r="O18" t="n">
-        <v>-4.23e-05</v>
+        <v>-6.341e-05</v>
       </c>
       <c r="P18" t="n">
-        <v>2.827e-26</v>
+        <v>4.856e-26</v>
       </c>
       <c r="Q18" t="n">
         <v>25</v>
@@ -1482,49 +1482,49 @@
         <v>0.84</v>
       </c>
       <c r="B19" t="n">
-        <v>9.981e-12</v>
+        <v>9.64e-12</v>
       </c>
       <c r="C19" t="n">
-        <v>8.466e-12</v>
+        <v>8.552e-12</v>
       </c>
       <c r="D19" t="n">
-        <v>9.224e-12</v>
+        <v>9.095999999999999e-12</v>
       </c>
       <c r="E19" t="n">
-        <v>5.905e-12</v>
+        <v>5.793e-12</v>
       </c>
       <c r="F19" t="n">
-        <v>4.944e-12</v>
+        <v>5.416e-12</v>
       </c>
       <c r="G19" t="n">
-        <v>5.425e-12</v>
+        <v>5.605e-12</v>
       </c>
       <c r="H19" t="n">
-        <v>6.136e-12</v>
+        <v>6.067e-12</v>
       </c>
       <c r="I19" t="n">
-        <v>5.773e-12</v>
+        <v>5.662e-12</v>
       </c>
       <c r="J19" t="n">
-        <v>5.954e-12</v>
+        <v>5.864e-12</v>
       </c>
       <c r="K19" t="n">
-        <v>4.638e-12</v>
+        <v>6.95e-12</v>
       </c>
       <c r="L19" t="n">
-        <v>5.183e-12</v>
+        <v>6.395e-12</v>
       </c>
       <c r="M19" t="n">
-        <v>4.91e-12</v>
+        <v>6.672e-12</v>
       </c>
       <c r="N19" t="n">
-        <v>2.551e-11</v>
+        <v>2.724e-11</v>
       </c>
       <c r="O19" t="n">
-        <v>-4.487e-05</v>
+        <v>-6.708e-05</v>
       </c>
       <c r="P19" t="n">
-        <v>2.921e-26</v>
+        <v>4.977000000000001e-26</v>
       </c>
       <c r="Q19" t="n">
         <v>25</v>
@@ -1538,49 +1538,49 @@
         <v>0.86</v>
       </c>
       <c r="B20" t="n">
-        <v>9.342e-12</v>
+        <v>9.523e-12</v>
       </c>
       <c r="C20" t="n">
-        <v>8.533e-12</v>
+        <v>8.431000000000001e-12</v>
       </c>
       <c r="D20" t="n">
-        <v>8.937999999999999e-12</v>
+        <v>8.976999999999999e-12</v>
       </c>
       <c r="E20" t="n">
-        <v>5.508e-12</v>
+        <v>5.711e-12</v>
       </c>
       <c r="F20" t="n">
-        <v>5.328e-12</v>
+        <v>5.331e-12</v>
       </c>
       <c r="G20" t="n">
-        <v>5.418e-12</v>
+        <v>5.521e-12</v>
       </c>
       <c r="H20" t="n">
-        <v>6.041e-12</v>
+        <v>5.97e-12</v>
       </c>
       <c r="I20" t="n">
-        <v>5.696e-12</v>
+        <v>5.569e-12</v>
       </c>
       <c r="J20" t="n">
-        <v>5.869e-12</v>
+        <v>5.77e-12</v>
       </c>
       <c r="K20" t="n">
-        <v>4.356e-12</v>
+        <v>6.851e-12</v>
       </c>
       <c r="L20" t="n">
-        <v>5.078e-12</v>
+        <v>6.294e-12</v>
       </c>
       <c r="M20" t="n">
-        <v>4.717e-12</v>
+        <v>6.573e-12</v>
       </c>
       <c r="N20" t="n">
-        <v>2.494e-11</v>
+        <v>2.684e-11</v>
       </c>
       <c r="O20" t="n">
-        <v>-4.762e-05</v>
+        <v>-7.088e-05</v>
       </c>
       <c r="P20" t="n">
-        <v>2.963e-26</v>
+        <v>5.106e-26</v>
       </c>
       <c r="Q20" t="n">
         <v>25</v>
@@ -1594,49 +1594,49 @@
         <v>0.88</v>
       </c>
       <c r="B21" t="n">
-        <v>9.717e-12</v>
+        <v>9.414e-12</v>
       </c>
       <c r="C21" t="n">
-        <v>8.559e-12</v>
+        <v>8.318000000000001e-12</v>
       </c>
       <c r="D21" t="n">
-        <v>9.137999999999999e-12</v>
+        <v>8.866e-12</v>
       </c>
       <c r="E21" t="n">
-        <v>5.288e-12</v>
+        <v>5.633e-12</v>
       </c>
       <c r="F21" t="n">
-        <v>4.855e-12</v>
+        <v>5.251e-12</v>
       </c>
       <c r="G21" t="n">
-        <v>5.072e-12</v>
+        <v>5.442e-12</v>
       </c>
       <c r="H21" t="n">
-        <v>5.977e-12</v>
+        <v>5.883e-12</v>
       </c>
       <c r="I21" t="n">
-        <v>5.634e-12</v>
+        <v>5.486e-12</v>
       </c>
       <c r="J21" t="n">
-        <v>5.806e-12</v>
+        <v>5.684e-12</v>
       </c>
       <c r="K21" t="n">
-        <v>4.407e-12</v>
+        <v>6.762e-12</v>
       </c>
       <c r="L21" t="n">
-        <v>5.069e-12</v>
+        <v>6.204e-12</v>
       </c>
       <c r="M21" t="n">
-        <v>4.738e-12</v>
+        <v>6.483e-12</v>
       </c>
       <c r="N21" t="n">
-        <v>2.475e-11</v>
+        <v>2.647e-11</v>
       </c>
       <c r="O21" t="n">
-        <v>-5.039e-05</v>
+        <v>-7.481e-05</v>
       </c>
       <c r="P21" t="n">
-        <v>3.088e-26</v>
+        <v>5.243e-26</v>
       </c>
       <c r="Q21" t="n">
         <v>25</v>
@@ -1650,49 +1650,49 @@
         <v>0.9</v>
       </c>
       <c r="B22" t="n">
-        <v>9.125000000000001e-12</v>
+        <v>9.305999999999999e-12</v>
       </c>
       <c r="C22" t="n">
-        <v>8.317e-12</v>
+        <v>8.211999999999999e-12</v>
       </c>
       <c r="D22" t="n">
-        <v>8.721000000000001e-12</v>
+        <v>8.759e-12</v>
       </c>
       <c r="E22" t="n">
-        <v>5.377e-12</v>
+        <v>5.558e-12</v>
       </c>
       <c r="F22" t="n">
-        <v>5.216e-12</v>
+        <v>5.178e-12</v>
       </c>
       <c r="G22" t="n">
-        <v>5.296e-12</v>
+        <v>5.368e-12</v>
       </c>
       <c r="H22" t="n">
-        <v>5.847e-12</v>
+        <v>5.805e-12</v>
       </c>
       <c r="I22" t="n">
-        <v>5.494e-12</v>
+        <v>5.406e-12</v>
       </c>
       <c r="J22" t="n">
-        <v>5.671e-12</v>
+        <v>5.605e-12</v>
       </c>
       <c r="K22" t="n">
-        <v>4.382e-12</v>
+        <v>6.677e-12</v>
       </c>
       <c r="L22" t="n">
-        <v>4.937e-12</v>
+        <v>6.12e-12</v>
       </c>
       <c r="M22" t="n">
-        <v>4.659e-12</v>
+        <v>6.398e-12</v>
       </c>
       <c r="N22" t="n">
-        <v>2.435e-11</v>
+        <v>2.613e-11</v>
       </c>
       <c r="O22" t="n">
-        <v>-5.332e-05</v>
+        <v>-7.888e-05</v>
       </c>
       <c r="P22" t="n">
-        <v>3.161e-26</v>
+        <v>5.386e-26</v>
       </c>
       <c r="Q22" t="n">
         <v>25</v>
@@ -1706,49 +1706,49 @@
         <v>0.92</v>
       </c>
       <c r="B23" t="n">
-        <v>9.263999999999999e-12</v>
+        <v>9.221e-12</v>
       </c>
       <c r="C23" t="n">
-        <v>8.062e-12</v>
+        <v>8.118000000000001e-12</v>
       </c>
       <c r="D23" t="n">
-        <v>8.663000000000001e-12</v>
+        <v>8.669999999999999e-12</v>
       </c>
       <c r="E23" t="n">
-        <v>5.615e-12</v>
+        <v>5.489e-12</v>
       </c>
       <c r="F23" t="n">
-        <v>4.865e-12</v>
+        <v>5.11e-12</v>
       </c>
       <c r="G23" t="n">
-        <v>5.24e-12</v>
+        <v>5.299e-12</v>
       </c>
       <c r="H23" t="n">
-        <v>5.86e-12</v>
+        <v>5.735e-12</v>
       </c>
       <c r="I23" t="n">
-        <v>5.398e-12</v>
+        <v>5.332e-12</v>
       </c>
       <c r="J23" t="n">
-        <v>5.629e-12</v>
+        <v>5.533e-12</v>
       </c>
       <c r="K23" t="n">
-        <v>4.317e-12</v>
+        <v>6.602e-12</v>
       </c>
       <c r="L23" t="n">
-        <v>4.84e-12</v>
+        <v>6.042e-12</v>
       </c>
       <c r="M23" t="n">
-        <v>4.579e-12</v>
+        <v>6.322e-12</v>
       </c>
       <c r="N23" t="n">
-        <v>2.411e-11</v>
+        <v>2.582e-11</v>
       </c>
       <c r="O23" t="n">
-        <v>-5.646e-05</v>
+        <v>-8.302e-05</v>
       </c>
       <c r="P23" t="n">
-        <v>3.282e-26</v>
+        <v>5.537e-26</v>
       </c>
       <c r="Q23" t="n">
         <v>25</v>
@@ -1762,49 +1762,49 @@
         <v>0.9399999999999999</v>
       </c>
       <c r="B24" t="n">
-        <v>9.586999999999999e-12</v>
+        <v>9.131000000000001e-12</v>
       </c>
       <c r="C24" t="n">
-        <v>8.056999999999999e-12</v>
+        <v>8.02e-12</v>
       </c>
       <c r="D24" t="n">
-        <v>8.821999999999999e-12</v>
+        <v>8.575e-12</v>
       </c>
       <c r="E24" t="n">
-        <v>5.372e-12</v>
+        <v>5.429e-12</v>
       </c>
       <c r="F24" t="n">
-        <v>4.602e-12</v>
+        <v>5.047e-12</v>
       </c>
       <c r="G24" t="n">
-        <v>4.987e-12</v>
+        <v>5.238e-12</v>
       </c>
       <c r="H24" t="n">
-        <v>5.797e-12</v>
+        <v>5.667e-12</v>
       </c>
       <c r="I24" t="n">
-        <v>5.255e-12</v>
+        <v>5.263e-12</v>
       </c>
       <c r="J24" t="n">
-        <v>5.526e-12</v>
+        <v>5.465e-12</v>
       </c>
       <c r="K24" t="n">
-        <v>4.282e-12</v>
+        <v>6.527e-12</v>
       </c>
       <c r="L24" t="n">
-        <v>4.765e-12</v>
+        <v>5.97e-12</v>
       </c>
       <c r="M24" t="n">
-        <v>4.524e-12</v>
+        <v>6.248e-12</v>
       </c>
       <c r="N24" t="n">
-        <v>2.386e-11</v>
+        <v>2.553e-11</v>
       </c>
       <c r="O24" t="n">
-        <v>-5.954e-05</v>
+        <v>-8.734e-05</v>
       </c>
       <c r="P24" t="n">
-        <v>3.389e-26</v>
+        <v>5.691e-26</v>
       </c>
       <c r="Q24" t="n">
         <v>25</v>
@@ -1818,49 +1818,49 @@
         <v>0.96</v>
       </c>
       <c r="B25" t="n">
-        <v>9.125000000000001e-12</v>
+        <v>9.047000000000001e-12</v>
       </c>
       <c r="C25" t="n">
-        <v>8.085e-12</v>
+        <v>7.937000000000001e-12</v>
       </c>
       <c r="D25" t="n">
-        <v>8.605000000000001e-12</v>
+        <v>8.492000000000001e-12</v>
       </c>
       <c r="E25" t="n">
-        <v>5.138e-12</v>
+        <v>5.365e-12</v>
       </c>
       <c r="F25" t="n">
-        <v>4.91e-12</v>
+        <v>4.987e-12</v>
       </c>
       <c r="G25" t="n">
-        <v>5.024e-12</v>
+        <v>5.176e-12</v>
       </c>
       <c r="H25" t="n">
-        <v>5.711e-12</v>
+        <v>5.597e-12</v>
       </c>
       <c r="I25" t="n">
-        <v>5.148e-12</v>
+        <v>5.199e-12</v>
       </c>
       <c r="J25" t="n">
-        <v>5.43e-12</v>
+        <v>5.398e-12</v>
       </c>
       <c r="K25" t="n">
-        <v>4.239e-12</v>
+        <v>6.46e-12</v>
       </c>
       <c r="L25" t="n">
-        <v>4.719e-12</v>
+        <v>5.9e-12</v>
       </c>
       <c r="M25" t="n">
-        <v>4.479e-12</v>
+        <v>6.18e-12</v>
       </c>
       <c r="N25" t="n">
-        <v>2.354e-11</v>
+        <v>2.525e-11</v>
       </c>
       <c r="O25" t="n">
-        <v>-6.279e-05</v>
+        <v>-9.176e-05</v>
       </c>
       <c r="P25" t="n">
-        <v>3.479e-26</v>
+        <v>5.849e-26</v>
       </c>
       <c r="Q25" t="n">
         <v>25</v>
@@ -1874,49 +1874,49 @@
         <v>0.98</v>
       </c>
       <c r="B26" t="n">
-        <v>8.833e-12</v>
+        <v>8.960000000000001e-12</v>
       </c>
       <c r="C26" t="n">
-        <v>8.022e-12</v>
+        <v>7.856e-12</v>
       </c>
       <c r="D26" t="n">
-        <v>8.427e-12</v>
+        <v>8.408000000000001e-12</v>
       </c>
       <c r="E26" t="n">
-        <v>5.339e-12</v>
+        <v>5.311e-12</v>
       </c>
       <c r="F26" t="n">
-        <v>5.029e-12</v>
+        <v>4.928e-12</v>
       </c>
       <c r="G26" t="n">
-        <v>5.184e-12</v>
+        <v>5.119e-12</v>
       </c>
       <c r="H26" t="n">
-        <v>5.642e-12</v>
+        <v>5.535e-12</v>
       </c>
       <c r="I26" t="n">
-        <v>5.28e-12</v>
+        <v>5.139e-12</v>
       </c>
       <c r="J26" t="n">
-        <v>5.461e-12</v>
+        <v>5.337e-12</v>
       </c>
       <c r="K26" t="n">
-        <v>4.183e-12</v>
+        <v>6.396e-12</v>
       </c>
       <c r="L26" t="n">
-        <v>4.643e-12</v>
+        <v>5.836e-12</v>
       </c>
       <c r="M26" t="n">
-        <v>4.413e-12</v>
+        <v>6.116e-12</v>
       </c>
       <c r="N26" t="n">
-        <v>2.349e-11</v>
+        <v>2.498e-11</v>
       </c>
       <c r="O26" t="n">
-        <v>-6.643999999999999e-05</v>
+        <v>-9.631e-05</v>
       </c>
       <c r="P26" t="n">
-        <v>3.665000000000001e-26</v>
+        <v>6.01e-26</v>
       </c>
       <c r="Q26" t="n">
         <v>25</v>
@@ -1930,54 +1930,1454 @@
         <v>1</v>
       </c>
       <c r="B27" t="n">
-        <v>8.905000000000001e-12</v>
+        <v>8.887e-12</v>
       </c>
       <c r="C27" t="n">
-        <v>7.918000000000001e-12</v>
+        <v>7.781e-12</v>
       </c>
       <c r="D27" t="n">
-        <v>8.411999999999999e-12</v>
+        <v>8.334000000000001e-12</v>
       </c>
       <c r="E27" t="n">
-        <v>5.044e-12</v>
+        <v>5.257e-12</v>
       </c>
       <c r="F27" t="n">
-        <v>4.896e-12</v>
+        <v>4.865e-12</v>
       </c>
       <c r="G27" t="n">
-        <v>4.97e-12</v>
+        <v>5.061e-12</v>
       </c>
       <c r="H27" t="n">
-        <v>5.574e-12</v>
+        <v>5.483e-12</v>
       </c>
       <c r="I27" t="n">
-        <v>4.972e-12</v>
+        <v>5.08e-12</v>
       </c>
       <c r="J27" t="n">
-        <v>5.273e-12</v>
+        <v>5.281e-12</v>
       </c>
       <c r="K27" t="n">
-        <v>4.218e-12</v>
+        <v>6.334e-12</v>
       </c>
       <c r="L27" t="n">
-        <v>4.556e-12</v>
+        <v>5.774e-12</v>
       </c>
       <c r="M27" t="n">
-        <v>4.387e-12</v>
+        <v>6.054e-12</v>
       </c>
       <c r="N27" t="n">
-        <v>2.304e-11</v>
+        <v>2.473e-11</v>
       </c>
       <c r="O27" t="n">
-        <v>-6.952999999999999e-05</v>
+        <v>-0.000101</v>
       </c>
       <c r="P27" t="n">
-        <v>3.692e-26</v>
+        <v>6.179e-26</v>
       </c>
       <c r="Q27" t="n">
         <v>25</v>
       </c>
       <c r="R27" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="28">
+      <c r="A28" t="n">
+        <v>1.02</v>
+      </c>
+      <c r="B28" t="n">
+        <v>8.837999999999999e-12</v>
+      </c>
+      <c r="C28" t="n">
+        <v>7.713e-12</v>
+      </c>
+      <c r="D28" t="n">
+        <v>8.275e-12</v>
+      </c>
+      <c r="E28" t="n">
+        <v>5.201e-12</v>
+      </c>
+      <c r="F28" t="n">
+        <v>4.816e-12</v>
+      </c>
+      <c r="G28" t="n">
+        <v>5.009e-12</v>
+      </c>
+      <c r="H28" t="n">
+        <v>5.429e-12</v>
+      </c>
+      <c r="I28" t="n">
+        <v>5.029e-12</v>
+      </c>
+      <c r="J28" t="n">
+        <v>5.229e-12</v>
+      </c>
+      <c r="K28" t="n">
+        <v>6.283e-12</v>
+      </c>
+      <c r="L28" t="n">
+        <v>5.722e-12</v>
+      </c>
+      <c r="M28" t="n">
+        <v>6.003e-12</v>
+      </c>
+      <c r="N28" t="n">
+        <v>2.452e-11</v>
+      </c>
+      <c r="O28" t="n">
+        <v>-0.0001059</v>
+      </c>
+      <c r="P28" t="n">
+        <v>6.366000000000001e-26</v>
+      </c>
+      <c r="Q28" t="n">
+        <v>25</v>
+      </c>
+      <c r="R28" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="29">
+      <c r="A29" t="n">
+        <v>1.04</v>
+      </c>
+      <c r="B29" t="n">
+        <v>8.775e-12</v>
+      </c>
+      <c r="C29" t="n">
+        <v>7.643999999999999e-12</v>
+      </c>
+      <c r="D29" t="n">
+        <v>8.208999999999999e-12</v>
+      </c>
+      <c r="E29" t="n">
+        <v>5.157e-12</v>
+      </c>
+      <c r="F29" t="n">
+        <v>4.767e-12</v>
+      </c>
+      <c r="G29" t="n">
+        <v>4.962e-12</v>
+      </c>
+      <c r="H29" t="n">
+        <v>5.378e-12</v>
+      </c>
+      <c r="I29" t="n">
+        <v>4.979e-12</v>
+      </c>
+      <c r="J29" t="n">
+        <v>5.178e-12</v>
+      </c>
+      <c r="K29" t="n">
+        <v>6.231e-12</v>
+      </c>
+      <c r="L29" t="n">
+        <v>5.67e-12</v>
+      </c>
+      <c r="M29" t="n">
+        <v>5.95e-12</v>
+      </c>
+      <c r="N29" t="n">
+        <v>2.43e-11</v>
+      </c>
+      <c r="O29" t="n">
+        <v>-0.000111</v>
+      </c>
+      <c r="P29" t="n">
+        <v>6.553e-26</v>
+      </c>
+      <c r="Q29" t="n">
+        <v>25</v>
+      </c>
+      <c r="R29" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="30">
+      <c r="A30" t="n">
+        <v>1.06</v>
+      </c>
+      <c r="B30" t="n">
+        <v>8.708999999999999e-12</v>
+      </c>
+      <c r="C30" t="n">
+        <v>7.582000000000001e-12</v>
+      </c>
+      <c r="D30" t="n">
+        <v>8.146e-12</v>
+      </c>
+      <c r="E30" t="n">
+        <v>5.113e-12</v>
+      </c>
+      <c r="F30" t="n">
+        <v>4.724e-12</v>
+      </c>
+      <c r="G30" t="n">
+        <v>4.919e-12</v>
+      </c>
+      <c r="H30" t="n">
+        <v>5.334e-12</v>
+      </c>
+      <c r="I30" t="n">
+        <v>4.931e-12</v>
+      </c>
+      <c r="J30" t="n">
+        <v>5.133e-12</v>
+      </c>
+      <c r="K30" t="n">
+        <v>6.183e-12</v>
+      </c>
+      <c r="L30" t="n">
+        <v>5.62e-12</v>
+      </c>
+      <c r="M30" t="n">
+        <v>5.901e-12</v>
+      </c>
+      <c r="N30" t="n">
+        <v>2.41e-11</v>
+      </c>
+      <c r="O30" t="n">
+        <v>-0.0001164</v>
+      </c>
+      <c r="P30" t="n">
+        <v>6.757e-26</v>
+      </c>
+      <c r="Q30" t="n">
+        <v>25</v>
+      </c>
+      <c r="R30" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="31">
+      <c r="A31" t="n">
+        <v>1.08</v>
+      </c>
+      <c r="B31" t="n">
+        <v>8.647000000000001e-12</v>
+      </c>
+      <c r="C31" t="n">
+        <v>7.527000000000001e-12</v>
+      </c>
+      <c r="D31" t="n">
+        <v>8.087e-12</v>
+      </c>
+      <c r="E31" t="n">
+        <v>5.072e-12</v>
+      </c>
+      <c r="F31" t="n">
+        <v>4.68e-12</v>
+      </c>
+      <c r="G31" t="n">
+        <v>4.876e-12</v>
+      </c>
+      <c r="H31" t="n">
+        <v>5.29e-12</v>
+      </c>
+      <c r="I31" t="n">
+        <v>4.888e-12</v>
+      </c>
+      <c r="J31" t="n">
+        <v>5.089e-12</v>
+      </c>
+      <c r="K31" t="n">
+        <v>6.135e-12</v>
+      </c>
+      <c r="L31" t="n">
+        <v>5.582e-12</v>
+      </c>
+      <c r="M31" t="n">
+        <v>5.859e-12</v>
+      </c>
+      <c r="N31" t="n">
+        <v>2.391e-11</v>
+      </c>
+      <c r="O31" t="n">
+        <v>-0.0001227</v>
+      </c>
+      <c r="P31" t="n">
+        <v>7.015000000000001e-26</v>
+      </c>
+      <c r="Q31" t="n">
+        <v>25</v>
+      </c>
+      <c r="R31" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="32">
+      <c r="A32" t="n">
+        <v>1.1</v>
+      </c>
+      <c r="B32" t="n">
+        <v>8.587e-12</v>
+      </c>
+      <c r="C32" t="n">
+        <v>7.466000000000001e-12</v>
+      </c>
+      <c r="D32" t="n">
+        <v>8.026e-12</v>
+      </c>
+      <c r="E32" t="n">
+        <v>5.03e-12</v>
+      </c>
+      <c r="F32" t="n">
+        <v>4.626e-12</v>
+      </c>
+      <c r="G32" t="n">
+        <v>4.828e-12</v>
+      </c>
+      <c r="H32" t="n">
+        <v>5.249e-12</v>
+      </c>
+      <c r="I32" t="n">
+        <v>4.844e-12</v>
+      </c>
+      <c r="J32" t="n">
+        <v>5.046e-12</v>
+      </c>
+      <c r="K32" t="n">
+        <v>6.089e-12</v>
+      </c>
+      <c r="L32" t="n">
+        <v>5.526e-12</v>
+      </c>
+      <c r="M32" t="n">
+        <v>5.807e-12</v>
+      </c>
+      <c r="N32" t="n">
+        <v>2.371e-11</v>
+      </c>
+      <c r="O32" t="n">
+        <v>-0.0001324</v>
+      </c>
+      <c r="P32" t="n">
+        <v>7.441000000000001e-26</v>
+      </c>
+      <c r="Q32" t="n">
+        <v>25</v>
+      </c>
+      <c r="R32" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="33">
+      <c r="A33" t="n">
+        <v>1.12</v>
+      </c>
+      <c r="B33" t="n">
+        <v>8.548e-12</v>
+      </c>
+      <c r="C33" t="n">
+        <v>7.408000000000001e-12</v>
+      </c>
+      <c r="D33" t="n">
+        <v>7.978e-12</v>
+      </c>
+      <c r="E33" t="n">
+        <v>4.994e-12</v>
+      </c>
+      <c r="F33" t="n">
+        <v>4.592e-12</v>
+      </c>
+      <c r="G33" t="n">
+        <v>4.793e-12</v>
+      </c>
+      <c r="H33" t="n">
+        <v>5.207e-12</v>
+      </c>
+      <c r="I33" t="n">
+        <v>4.799e-12</v>
+      </c>
+      <c r="J33" t="n">
+        <v>5.003e-12</v>
+      </c>
+      <c r="K33" t="n">
+        <v>6.044e-12</v>
+      </c>
+      <c r="L33" t="n">
+        <v>5.476e-12</v>
+      </c>
+      <c r="M33" t="n">
+        <v>5.76e-12</v>
+      </c>
+      <c r="N33" t="n">
+        <v>2.353e-11</v>
+      </c>
+      <c r="O33" t="n">
+        <v>-0.0001528</v>
+      </c>
+      <c r="P33" t="n">
+        <v>8.463e-26</v>
+      </c>
+      <c r="Q33" t="n">
+        <v>25</v>
+      </c>
+      <c r="R33" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="34">
+      <c r="A34" t="n">
+        <v>1.14</v>
+      </c>
+      <c r="B34" t="n">
+        <v>8.49e-12</v>
+      </c>
+      <c r="C34" t="n">
+        <v>7.343999999999999e-12</v>
+      </c>
+      <c r="D34" t="n">
+        <v>7.917e-12</v>
+      </c>
+      <c r="E34" t="n">
+        <v>4.959e-12</v>
+      </c>
+      <c r="F34" t="n">
+        <v>4.549e-12</v>
+      </c>
+      <c r="G34" t="n">
+        <v>4.754e-12</v>
+      </c>
+      <c r="H34" t="n">
+        <v>5.161e-12</v>
+      </c>
+      <c r="I34" t="n">
+        <v>4.747e-12</v>
+      </c>
+      <c r="J34" t="n">
+        <v>4.954e-12</v>
+      </c>
+      <c r="K34" t="n">
+        <v>5.993e-12</v>
+      </c>
+      <c r="L34" t="n">
+        <v>5.416e-12</v>
+      </c>
+      <c r="M34" t="n">
+        <v>5.705e-12</v>
+      </c>
+      <c r="N34" t="n">
+        <v>2.333e-11</v>
+      </c>
+      <c r="O34" t="n">
+        <v>-0.0002014</v>
+      </c>
+      <c r="P34" t="n">
+        <v>1.096e-25</v>
+      </c>
+      <c r="Q34" t="n">
+        <v>25</v>
+      </c>
+      <c r="R34" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="35">
+      <c r="A35" t="n">
+        <v>1.16</v>
+      </c>
+      <c r="B35" t="n">
+        <v>8.427e-12</v>
+      </c>
+      <c r="C35" t="n">
+        <v>7.275e-12</v>
+      </c>
+      <c r="D35" t="n">
+        <v>7.851e-12</v>
+      </c>
+      <c r="E35" t="n">
+        <v>4.918e-12</v>
+      </c>
+      <c r="F35" t="n">
+        <v>4.498e-12</v>
+      </c>
+      <c r="G35" t="n">
+        <v>4.708e-12</v>
+      </c>
+      <c r="H35" t="n">
+        <v>5.109e-12</v>
+      </c>
+      <c r="I35" t="n">
+        <v>4.686e-12</v>
+      </c>
+      <c r="J35" t="n">
+        <v>4.897e-12</v>
+      </c>
+      <c r="K35" t="n">
+        <v>5.93e-12</v>
+      </c>
+      <c r="L35" t="n">
+        <v>5.349e-12</v>
+      </c>
+      <c r="M35" t="n">
+        <v>5.639e-12</v>
+      </c>
+      <c r="N35" t="n">
+        <v>2.31e-11</v>
+      </c>
+      <c r="O35" t="n">
+        <v>-0.0002962</v>
+      </c>
+      <c r="P35" t="n">
+        <v>1.58e-25</v>
+      </c>
+      <c r="Q35" t="n">
+        <v>25</v>
+      </c>
+      <c r="R35" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="36">
+      <c r="A36" t="n">
+        <v>1.18</v>
+      </c>
+      <c r="B36" t="n">
+        <v>8.343e-12</v>
+      </c>
+      <c r="C36" t="n">
+        <v>7.193e-12</v>
+      </c>
+      <c r="D36" t="n">
+        <v>7.768e-12</v>
+      </c>
+      <c r="E36" t="n">
+        <v>4.879e-12</v>
+      </c>
+      <c r="F36" t="n">
+        <v>4.456e-12</v>
+      </c>
+      <c r="G36" t="n">
+        <v>4.667e-12</v>
+      </c>
+      <c r="H36" t="n">
+        <v>5.054e-12</v>
+      </c>
+      <c r="I36" t="n">
+        <v>4.62e-12</v>
+      </c>
+      <c r="J36" t="n">
+        <v>4.837e-12</v>
+      </c>
+      <c r="K36" t="n">
+        <v>5.856e-12</v>
+      </c>
+      <c r="L36" t="n">
+        <v>5.267e-12</v>
+      </c>
+      <c r="M36" t="n">
+        <v>5.561e-12</v>
+      </c>
+      <c r="N36" t="n">
+        <v>2.283e-11</v>
+      </c>
+      <c r="O36" t="n">
+        <v>-0.000438</v>
+      </c>
+      <c r="P36" t="n">
+        <v>2.284e-25</v>
+      </c>
+      <c r="Q36" t="n">
+        <v>25</v>
+      </c>
+      <c r="R36" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="37">
+      <c r="A37" t="n">
+        <v>1.2</v>
+      </c>
+      <c r="B37" t="n">
+        <v>8.273000000000001e-12</v>
+      </c>
+      <c r="C37" t="n">
+        <v>7.113e-12</v>
+      </c>
+      <c r="D37" t="n">
+        <v>7.693e-12</v>
+      </c>
+      <c r="E37" t="n">
+        <v>4.837e-12</v>
+      </c>
+      <c r="F37" t="n">
+        <v>4.404e-12</v>
+      </c>
+      <c r="G37" t="n">
+        <v>4.62e-12</v>
+      </c>
+      <c r="H37" t="n">
+        <v>4.996e-12</v>
+      </c>
+      <c r="I37" t="n">
+        <v>4.554e-12</v>
+      </c>
+      <c r="J37" t="n">
+        <v>4.775e-12</v>
+      </c>
+      <c r="K37" t="n">
+        <v>5.774e-12</v>
+      </c>
+      <c r="L37" t="n">
+        <v>5.181e-12</v>
+      </c>
+      <c r="M37" t="n">
+        <v>5.478e-12</v>
+      </c>
+      <c r="N37" t="n">
+        <v>2.257e-11</v>
+      </c>
+      <c r="O37" t="n">
+        <v>-0.000617</v>
+      </c>
+      <c r="P37" t="n">
+        <v>3.142e-25</v>
+      </c>
+      <c r="Q37" t="n">
+        <v>25</v>
+      </c>
+      <c r="R37" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="38">
+      <c r="A38" t="n">
+        <v>1.22</v>
+      </c>
+      <c r="B38" t="n">
+        <v>8.198999999999999e-12</v>
+      </c>
+      <c r="C38" t="n">
+        <v>7.027e-12</v>
+      </c>
+      <c r="D38" t="n">
+        <v>7.613e-12</v>
+      </c>
+      <c r="E38" t="n">
+        <v>4.799e-12</v>
+      </c>
+      <c r="F38" t="n">
+        <v>4.349e-12</v>
+      </c>
+      <c r="G38" t="n">
+        <v>4.574e-12</v>
+      </c>
+      <c r="H38" t="n">
+        <v>4.937e-12</v>
+      </c>
+      <c r="I38" t="n">
+        <v>4.49e-12</v>
+      </c>
+      <c r="J38" t="n">
+        <v>4.713e-12</v>
+      </c>
+      <c r="K38" t="n">
+        <v>5.694e-12</v>
+      </c>
+      <c r="L38" t="n">
+        <v>5.098e-12</v>
+      </c>
+      <c r="M38" t="n">
+        <v>5.396e-12</v>
+      </c>
+      <c r="N38" t="n">
+        <v>2.23e-11</v>
+      </c>
+      <c r="O38" t="n">
+        <v>-0.0008254</v>
+      </c>
+      <c r="P38" t="n">
+        <v>4.103e-25</v>
+      </c>
+      <c r="Q38" t="n">
+        <v>25</v>
+      </c>
+      <c r="R38" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="39">
+      <c r="A39" t="n">
+        <v>1.24</v>
+      </c>
+      <c r="B39" t="n">
+        <v>8.124999999999999e-12</v>
+      </c>
+      <c r="C39" t="n">
+        <v>6.948e-12</v>
+      </c>
+      <c r="D39" t="n">
+        <v>7.537000000000001e-12</v>
+      </c>
+      <c r="E39" t="n">
+        <v>4.748e-12</v>
+      </c>
+      <c r="F39" t="n">
+        <v>4.299e-12</v>
+      </c>
+      <c r="G39" t="n">
+        <v>4.523e-12</v>
+      </c>
+      <c r="H39" t="n">
+        <v>4.88e-12</v>
+      </c>
+      <c r="I39" t="n">
+        <v>4.426e-12</v>
+      </c>
+      <c r="J39" t="n">
+        <v>4.653e-12</v>
+      </c>
+      <c r="K39" t="n">
+        <v>5.609e-12</v>
+      </c>
+      <c r="L39" t="n">
+        <v>5.022e-12</v>
+      </c>
+      <c r="M39" t="n">
+        <v>5.316e-12</v>
+      </c>
+      <c r="N39" t="n">
+        <v>2.203e-11</v>
+      </c>
+      <c r="O39" t="n">
+        <v>-0.001063</v>
+      </c>
+      <c r="P39" t="n">
+        <v>5.157e-25</v>
+      </c>
+      <c r="Q39" t="n">
+        <v>25</v>
+      </c>
+      <c r="R39" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="40">
+      <c r="A40" t="n">
+        <v>1.26</v>
+      </c>
+      <c r="B40" t="n">
+        <v>8.049e-12</v>
+      </c>
+      <c r="C40" t="n">
+        <v>6.867e-12</v>
+      </c>
+      <c r="D40" t="n">
+        <v>7.458e-12</v>
+      </c>
+      <c r="E40" t="n">
+        <v>4.712e-12</v>
+      </c>
+      <c r="F40" t="n">
+        <v>4.254e-12</v>
+      </c>
+      <c r="G40" t="n">
+        <v>4.483e-12</v>
+      </c>
+      <c r="H40" t="n">
+        <v>4.822e-12</v>
+      </c>
+      <c r="I40" t="n">
+        <v>4.368e-12</v>
+      </c>
+      <c r="J40" t="n">
+        <v>4.595e-12</v>
+      </c>
+      <c r="K40" t="n">
+        <v>5.519e-12</v>
+      </c>
+      <c r="L40" t="n">
+        <v>4.924e-12</v>
+      </c>
+      <c r="M40" t="n">
+        <v>5.222e-12</v>
+      </c>
+      <c r="N40" t="n">
+        <v>2.176e-11</v>
+      </c>
+      <c r="O40" t="n">
+        <v>-0.00134</v>
+      </c>
+      <c r="P40" t="n">
+        <v>6.342e-25</v>
+      </c>
+      <c r="Q40" t="n">
+        <v>25</v>
+      </c>
+      <c r="R40" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="41">
+      <c r="A41" t="n">
+        <v>1.28</v>
+      </c>
+      <c r="B41" t="n">
+        <v>7.977e-12</v>
+      </c>
+      <c r="C41" t="n">
+        <v>6.789e-12</v>
+      </c>
+      <c r="D41" t="n">
+        <v>7.383e-12</v>
+      </c>
+      <c r="E41" t="n">
+        <v>4.665e-12</v>
+      </c>
+      <c r="F41" t="n">
+        <v>4.201e-12</v>
+      </c>
+      <c r="G41" t="n">
+        <v>4.433e-12</v>
+      </c>
+      <c r="H41" t="n">
+        <v>4.769e-12</v>
+      </c>
+      <c r="I41" t="n">
+        <v>4.311e-12</v>
+      </c>
+      <c r="J41" t="n">
+        <v>4.54e-12</v>
+      </c>
+      <c r="K41" t="n">
+        <v>5.43e-12</v>
+      </c>
+      <c r="L41" t="n">
+        <v>4.835e-12</v>
+      </c>
+      <c r="M41" t="n">
+        <v>5.132e-12</v>
+      </c>
+      <c r="N41" t="n">
+        <v>2.149e-11</v>
+      </c>
+      <c r="O41" t="n">
+        <v>-0.001693</v>
+      </c>
+      <c r="P41" t="n">
+        <v>7.818e-25</v>
+      </c>
+      <c r="Q41" t="n">
+        <v>25</v>
+      </c>
+      <c r="R41" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="42">
+      <c r="A42" t="n">
+        <v>1.3</v>
+      </c>
+      <c r="B42" t="n">
+        <v>7.901999999999999e-12</v>
+      </c>
+      <c r="C42" t="n">
+        <v>6.684e-12</v>
+      </c>
+      <c r="D42" t="n">
+        <v>7.293e-12</v>
+      </c>
+      <c r="E42" t="n">
+        <v>4.634e-12</v>
+      </c>
+      <c r="F42" t="n">
+        <v>4.151e-12</v>
+      </c>
+      <c r="G42" t="n">
+        <v>4.392e-12</v>
+      </c>
+      <c r="H42" t="n">
+        <v>4.714e-12</v>
+      </c>
+      <c r="I42" t="n">
+        <v>4.256e-12</v>
+      </c>
+      <c r="J42" t="n">
+        <v>4.485e-12</v>
+      </c>
+      <c r="K42" t="n">
+        <v>5.337e-12</v>
+      </c>
+      <c r="L42" t="n">
+        <v>4.748e-12</v>
+      </c>
+      <c r="M42" t="n">
+        <v>5.043e-12</v>
+      </c>
+      <c r="N42" t="n">
+        <v>2.121e-11</v>
+      </c>
+      <c r="O42" t="n">
+        <v>-0.002225</v>
+      </c>
+      <c r="P42" t="n">
+        <v>1.001e-24</v>
+      </c>
+      <c r="Q42" t="n">
+        <v>25</v>
+      </c>
+      <c r="R42" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="43">
+      <c r="A43" t="n">
+        <v>1.32</v>
+      </c>
+      <c r="B43" t="n">
+        <v>7.834000000000001e-12</v>
+      </c>
+      <c r="C43" t="n">
+        <v>6.639e-12</v>
+      </c>
+      <c r="D43" t="n">
+        <v>7.236e-12</v>
+      </c>
+      <c r="E43" t="n">
+        <v>4.571e-12</v>
+      </c>
+      <c r="F43" t="n">
+        <v>4.099e-12</v>
+      </c>
+      <c r="G43" t="n">
+        <v>4.335e-12</v>
+      </c>
+      <c r="H43" t="n">
+        <v>4.66e-12</v>
+      </c>
+      <c r="I43" t="n">
+        <v>4.207e-12</v>
+      </c>
+      <c r="J43" t="n">
+        <v>4.434e-12</v>
+      </c>
+      <c r="K43" t="n">
+        <v>5.247e-12</v>
+      </c>
+      <c r="L43" t="n">
+        <v>4.665e-12</v>
+      </c>
+      <c r="M43" t="n">
+        <v>4.956e-12</v>
+      </c>
+      <c r="N43" t="n">
+        <v>2.096e-11</v>
+      </c>
+      <c r="O43" t="n">
+        <v>-0.003212</v>
+      </c>
+      <c r="P43" t="n">
+        <v>1.411e-24</v>
+      </c>
+      <c r="Q43" t="n">
+        <v>25</v>
+      </c>
+      <c r="R43" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="44">
+      <c r="A44" t="n">
+        <v>1.34</v>
+      </c>
+      <c r="B44" t="n">
+        <v>7.755e-12</v>
+      </c>
+      <c r="C44" t="n">
+        <v>6.569e-12</v>
+      </c>
+      <c r="D44" t="n">
+        <v>7.162e-12</v>
+      </c>
+      <c r="E44" t="n">
+        <v>4.523e-12</v>
+      </c>
+      <c r="F44" t="n">
+        <v>4.056e-12</v>
+      </c>
+      <c r="G44" t="n">
+        <v>4.29e-12</v>
+      </c>
+      <c r="H44" t="n">
+        <v>4.608e-12</v>
+      </c>
+      <c r="I44" t="n">
+        <v>4.157e-12</v>
+      </c>
+      <c r="J44" t="n">
+        <v>4.383e-12</v>
+      </c>
+      <c r="K44" t="n">
+        <v>5.157e-12</v>
+      </c>
+      <c r="L44" t="n">
+        <v>4.58e-12</v>
+      </c>
+      <c r="M44" t="n">
+        <v>4.868e-12</v>
+      </c>
+      <c r="N44" t="n">
+        <v>2.07e-11</v>
+      </c>
+      <c r="O44" t="n">
+        <v>-0.005387</v>
+      </c>
+      <c r="P44" t="n">
+        <v>2.309e-24</v>
+      </c>
+      <c r="Q44" t="n">
+        <v>25</v>
+      </c>
+      <c r="R44" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="45">
+      <c r="A45" t="n">
+        <v>1.36</v>
+      </c>
+      <c r="B45" t="n">
+        <v>7.692000000000001e-12</v>
+      </c>
+      <c r="C45" t="n">
+        <v>6.493e-12</v>
+      </c>
+      <c r="D45" t="n">
+        <v>7.093e-12</v>
+      </c>
+      <c r="E45" t="n">
+        <v>4.485e-12</v>
+      </c>
+      <c r="F45" t="n">
+        <v>4e-12</v>
+      </c>
+      <c r="G45" t="n">
+        <v>4.242e-12</v>
+      </c>
+      <c r="H45" t="n">
+        <v>4.562e-12</v>
+      </c>
+      <c r="I45" t="n">
+        <v>4.106e-12</v>
+      </c>
+      <c r="J45" t="n">
+        <v>4.334e-12</v>
+      </c>
+      <c r="K45" t="n">
+        <v>5.068e-12</v>
+      </c>
+      <c r="L45" t="n">
+        <v>4.496e-12</v>
+      </c>
+      <c r="M45" t="n">
+        <v>4.782e-12</v>
+      </c>
+      <c r="N45" t="n">
+        <v>2.045e-11</v>
+      </c>
+      <c r="O45" t="n">
+        <v>-0.0107</v>
+      </c>
+      <c r="P45" t="n">
+        <v>4.473e-24</v>
+      </c>
+      <c r="Q45" t="n">
+        <v>25</v>
+      </c>
+      <c r="R45" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="46">
+      <c r="A46" t="n">
+        <v>1.38</v>
+      </c>
+      <c r="B46" t="n">
+        <v>7.626e-12</v>
+      </c>
+      <c r="C46" t="n">
+        <v>6.422e-12</v>
+      </c>
+      <c r="D46" t="n">
+        <v>7.024e-12</v>
+      </c>
+      <c r="E46" t="n">
+        <v>4.442e-12</v>
+      </c>
+      <c r="F46" t="n">
+        <v>3.953e-12</v>
+      </c>
+      <c r="G46" t="n">
+        <v>4.197e-12</v>
+      </c>
+      <c r="H46" t="n">
+        <v>4.506e-12</v>
+      </c>
+      <c r="I46" t="n">
+        <v>4.057e-12</v>
+      </c>
+      <c r="J46" t="n">
+        <v>4.282e-12</v>
+      </c>
+      <c r="K46" t="n">
+        <v>4.985e-12</v>
+      </c>
+      <c r="L46" t="n">
+        <v>4.415e-12</v>
+      </c>
+      <c r="M46" t="n">
+        <v>4.7e-12</v>
+      </c>
+      <c r="N46" t="n">
+        <v>2.02e-11</v>
+      </c>
+      <c r="O46" t="n">
+        <v>-0.02427</v>
+      </c>
+      <c r="P46" t="n">
+        <v>9.906e-24</v>
+      </c>
+      <c r="Q46" t="n">
+        <v>25</v>
+      </c>
+      <c r="R46" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="47">
+      <c r="A47" t="n">
+        <v>1.4</v>
+      </c>
+      <c r="B47" t="n">
+        <v>7.556999999999999e-12</v>
+      </c>
+      <c r="C47" t="n">
+        <v>6.335e-12</v>
+      </c>
+      <c r="D47" t="n">
+        <v>6.946e-12</v>
+      </c>
+      <c r="E47" t="n">
+        <v>4.403e-12</v>
+      </c>
+      <c r="F47" t="n">
+        <v>3.908e-12</v>
+      </c>
+      <c r="G47" t="n">
+        <v>4.156e-12</v>
+      </c>
+      <c r="H47" t="n">
+        <v>4.463e-12</v>
+      </c>
+      <c r="I47" t="n">
+        <v>4.011e-12</v>
+      </c>
+      <c r="J47" t="n">
+        <v>4.237e-12</v>
+      </c>
+      <c r="K47" t="n">
+        <v>4.903e-12</v>
+      </c>
+      <c r="L47" t="n">
+        <v>4.333e-12</v>
+      </c>
+      <c r="M47" t="n">
+        <v>4.618e-12</v>
+      </c>
+      <c r="N47" t="n">
+        <v>1.996e-11</v>
+      </c>
+      <c r="O47" t="n">
+        <v>-0.05963</v>
+      </c>
+      <c r="P47" t="n">
+        <v>2.375e-23</v>
+      </c>
+      <c r="Q47" t="n">
+        <v>25</v>
+      </c>
+      <c r="R47" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="48">
+      <c r="A48" t="n">
+        <v>1.42</v>
+      </c>
+      <c r="B48" t="n">
+        <v>7.482000000000001e-12</v>
+      </c>
+      <c r="C48" t="n">
+        <v>6.276e-12</v>
+      </c>
+      <c r="D48" t="n">
+        <v>6.879e-12</v>
+      </c>
+      <c r="E48" t="n">
+        <v>4.352e-12</v>
+      </c>
+      <c r="F48" t="n">
+        <v>3.863e-12</v>
+      </c>
+      <c r="G48" t="n">
+        <v>4.107e-12</v>
+      </c>
+      <c r="H48" t="n">
+        <v>4.415e-12</v>
+      </c>
+      <c r="I48" t="n">
+        <v>3.968e-12</v>
+      </c>
+      <c r="J48" t="n">
+        <v>4.191e-12</v>
+      </c>
+      <c r="K48" t="n">
+        <v>4.815e-12</v>
+      </c>
+      <c r="L48" t="n">
+        <v>4.253e-12</v>
+      </c>
+      <c r="M48" t="n">
+        <v>4.534e-12</v>
+      </c>
+      <c r="N48" t="n">
+        <v>1.971e-11</v>
+      </c>
+      <c r="O48" t="n">
+        <v>-0.1523</v>
+      </c>
+      <c r="P48" t="n">
+        <v>5.917999999999999e-23</v>
+      </c>
+      <c r="Q48" t="n">
+        <v>25</v>
+      </c>
+      <c r="R48" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="49">
+      <c r="A49" t="n">
+        <v>1.44</v>
+      </c>
+      <c r="B49" t="n">
+        <v>7.425e-12</v>
+      </c>
+      <c r="C49" t="n">
+        <v>6.211e-12</v>
+      </c>
+      <c r="D49" t="n">
+        <v>6.818e-12</v>
+      </c>
+      <c r="E49" t="n">
+        <v>4.307e-12</v>
+      </c>
+      <c r="F49" t="n">
+        <v>3.81e-12</v>
+      </c>
+      <c r="G49" t="n">
+        <v>4.059e-12</v>
+      </c>
+      <c r="H49" t="n">
+        <v>4.368e-12</v>
+      </c>
+      <c r="I49" t="n">
+        <v>3.92e-12</v>
+      </c>
+      <c r="J49" t="n">
+        <v>4.144e-12</v>
+      </c>
+      <c r="K49" t="n">
+        <v>4.745e-12</v>
+      </c>
+      <c r="L49" t="n">
+        <v>4.176e-12</v>
+      </c>
+      <c r="M49" t="n">
+        <v>4.46e-12</v>
+      </c>
+      <c r="N49" t="n">
+        <v>1.948e-11</v>
+      </c>
+      <c r="O49" t="n">
+        <v>-0.3956</v>
+      </c>
+      <c r="P49" t="n">
+        <v>1.501e-22</v>
+      </c>
+      <c r="Q49" t="n">
+        <v>25</v>
+      </c>
+      <c r="R49" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="50">
+      <c r="A50" t="n">
+        <v>1.46</v>
+      </c>
+      <c r="B50" t="n">
+        <v>7.351e-12</v>
+      </c>
+      <c r="C50" t="n">
+        <v>6.139e-12</v>
+      </c>
+      <c r="D50" t="n">
+        <v>6.745e-12</v>
+      </c>
+      <c r="E50" t="n">
+        <v>4.265e-12</v>
+      </c>
+      <c r="F50" t="n">
+        <v>3.775e-12</v>
+      </c>
+      <c r="G50" t="n">
+        <v>4.02e-12</v>
+      </c>
+      <c r="H50" t="n">
+        <v>4.325e-12</v>
+      </c>
+      <c r="I50" t="n">
+        <v>3.878e-12</v>
+      </c>
+      <c r="J50" t="n">
+        <v>4.101e-12</v>
+      </c>
+      <c r="K50" t="n">
+        <v>4.666e-12</v>
+      </c>
+      <c r="L50" t="n">
+        <v>4.102e-12</v>
+      </c>
+      <c r="M50" t="n">
+        <v>4.384e-12</v>
+      </c>
+      <c r="N50" t="n">
+        <v>1.925e-11</v>
+      </c>
+      <c r="O50" t="n">
+        <v>-1.0341</v>
+      </c>
+      <c r="P50" t="n">
+        <v>3.831999999999999e-22</v>
+      </c>
+      <c r="Q50" t="n">
+        <v>25</v>
+      </c>
+      <c r="R50" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="51">
+      <c r="A51" t="n">
+        <v>1.48</v>
+      </c>
+      <c r="B51" t="n">
+        <v>7.275999999999999e-12</v>
+      </c>
+      <c r="C51" t="n">
+        <v>6.079e-12</v>
+      </c>
+      <c r="D51" t="n">
+        <v>6.678e-12</v>
+      </c>
+      <c r="E51" t="n">
+        <v>4.226e-12</v>
+      </c>
+      <c r="F51" t="n">
+        <v>3.731e-12</v>
+      </c>
+      <c r="G51" t="n">
+        <v>3.978e-12</v>
+      </c>
+      <c r="H51" t="n">
+        <v>4.281e-12</v>
+      </c>
+      <c r="I51" t="n">
+        <v>3.832e-12</v>
+      </c>
+      <c r="J51" t="n">
+        <v>4.056e-12</v>
+      </c>
+      <c r="K51" t="n">
+        <v>4.595e-12</v>
+      </c>
+      <c r="L51" t="n">
+        <v>4.027e-12</v>
+      </c>
+      <c r="M51" t="n">
+        <v>4.311e-12</v>
+      </c>
+      <c r="N51" t="n">
+        <v>1.902e-11</v>
+      </c>
+      <c r="O51" t="n">
+        <v>-2.7087</v>
+      </c>
+      <c r="P51" t="n">
+        <v>9.802e-22</v>
+      </c>
+      <c r="Q51" t="n">
+        <v>25</v>
+      </c>
+      <c r="R51" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="52">
+      <c r="A52" t="n">
+        <v>1.5</v>
+      </c>
+      <c r="B52" t="n">
+        <v>7.206e-12</v>
+      </c>
+      <c r="C52" t="n">
+        <v>6.027e-12</v>
+      </c>
+      <c r="D52" t="n">
+        <v>6.616e-12</v>
+      </c>
+      <c r="E52" t="n">
+        <v>4.176e-12</v>
+      </c>
+      <c r="F52" t="n">
+        <v>3.69e-12</v>
+      </c>
+      <c r="G52" t="n">
+        <v>3.933e-12</v>
+      </c>
+      <c r="H52" t="n">
+        <v>4.233e-12</v>
+      </c>
+      <c r="I52" t="n">
+        <v>3.79e-12</v>
+      </c>
+      <c r="J52" t="n">
+        <v>4.012e-12</v>
+      </c>
+      <c r="K52" t="n">
+        <v>4.522e-12</v>
+      </c>
+      <c r="L52" t="n">
+        <v>3.953e-12</v>
+      </c>
+      <c r="M52" t="n">
+        <v>4.238e-12</v>
+      </c>
+      <c r="N52" t="n">
+        <v>1.88e-11</v>
+      </c>
+      <c r="O52" t="n">
+        <v>-7.0934</v>
+      </c>
+      <c r="P52" t="n">
+        <v>2.507e-21</v>
+      </c>
+      <c r="Q52" t="n">
+        <v>25</v>
+      </c>
+      <c r="R52" t="n">
         <v>1</v>
       </c>
     </row>

</xml_diff>